<commit_message>
Refactor thesis panel member handling and improve URL validation
- Updated HandledThesisModal and ThesisSubmissionCard to use individual panel member fields instead of a combined list.
- Modified BookmarksClient to display panel members correctly.
- Enhanced ConfirmModal to include a thesis document link input with validation.
- Adjusted InputPanel to reflect changes in research title and overview terminology.
- Added URL input in ResendModal for thesis-related links.
- Updated UploadThesisModal to manage individual panel member inputs.
- Improved ConfirmationModal to sort advisers based on recommendations.
- Refined RequestCard to display thesis URLs and adjusted button functionalities.
- Updated various types and hooks to accommodate new panel member structure and thesis URL handling.
- Created utility functions for URL validation and adviser sorting.
- Corrected email templates to reflect updated contact information.
</commit_message>
<xml_diff>
--- a/data/new_theses.xlsx
+++ b/data/new_theses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrroy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644DF6A7-2002-49AB-B822-329288203E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44B2B59-F045-457B-96E9-3AE967B5B00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4B055C28-C125-4A87-9575-404E4D2C58AE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4304" uniqueCount="2233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4304" uniqueCount="2231">
   <si>
     <t>no.</t>
   </si>
@@ -6006,9 +6006,6 @@
     <t>Archie O. Pachica, Naive, Al-Monte Vince M. Calo</t>
   </si>
   <si>
-    <t>Arlene A. Arlene A. Baldelovar</t>
-  </si>
-  <si>
     <t>Sabanal, Arlene A. Baldelovar</t>
   </si>
   <si>
@@ -6378,12 +6375,6 @@
     <t>Ma. Esther B. Chio, Estrera, Al-Monte Vince M. Calo</t>
   </si>
   <si>
-    <t>Ma. Esther B. Chio, Arlene A. Arlene A. Baldelovar, Sabanal</t>
-  </si>
-  <si>
-    <t>Arlene A. Arlene A. Baldelovar, Ma. Esther B. Chio, Sabanal</t>
-  </si>
-  <si>
     <t>Jay Noel N. Rojo, Maricel A. Esclamado, Baconguis</t>
   </si>
   <si>
@@ -6405,9 +6396,6 @@
     <t>Dela Cruz, Baconguis, Maricel A. Esclamado</t>
   </si>
   <si>
-    <t>Maricel A. Esclamado, M.</t>
-  </si>
-  <si>
     <t>Maricel A. Esclamado, J., Dela Cruz, Jay Noel N. Rojo</t>
   </si>
   <si>
@@ -6807,15 +6795,9 @@
     <t>Petal May M. Dal, Edulsa, Jocelyn L. Garrido</t>
   </si>
   <si>
-    <t>Petal May M. Dal, Arlene A. Arlene A. Baldelovar, Sabanal</t>
-  </si>
-  <si>
     <t>Love Jhoye M. Raboy, Jomar C. Llevado, Petal May M. Dal</t>
   </si>
   <si>
-    <t>Legara, Arlene A. Arlene A. Baldelovar, Petal May M. Dal</t>
-  </si>
-  <si>
     <t>Petal May M. Dal, Jc Vanny Mill A. Saledaien, John Benedict L. Bernardo</t>
   </si>
   <si>
@@ -6976,6 +6958,18 @@
   </si>
   <si>
     <t>Ulrich Lee F. Uy, Junar A. Landicho, John Benedict L. Bernardo</t>
+  </si>
+  <si>
+    <t>Petal May M. Dal, Arlene A. Baldelovar, Sabanal</t>
+  </si>
+  <si>
+    <t>Ma. Esther B. Chio, Arlene A. Baldelovar, Sabanal</t>
+  </si>
+  <si>
+    <t>Arlene A. Baldelovar, Ma. Esther B. Chio, Sabanal</t>
+  </si>
+  <si>
+    <t>Legara, Arlene A. Baldelovar, Petal May M. Dal</t>
   </si>
 </sst>
 </file>
@@ -7590,8 +7584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7AC19F-84D5-45F1-881A-961C86843A2F}">
   <dimension ref="A1:K399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="D293" sqref="D293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7645,7 +7639,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>11</v>
@@ -7680,7 +7674,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>17</v>
@@ -7715,7 +7709,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>21</v>
@@ -7750,7 +7744,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>24</v>
@@ -7785,7 +7779,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
@@ -7820,7 +7814,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>30</v>
@@ -7855,7 +7849,7 @@
         <v>1614</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>33</v>
@@ -7890,7 +7884,7 @@
         <v>1614</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>36</v>
@@ -7925,7 +7919,7 @@
         <v>1614</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>39</v>
@@ -7960,7 +7954,7 @@
         <v>1614</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>42</v>
@@ -7995,7 +7989,7 @@
         <v>1614</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>45</v>
@@ -8030,7 +8024,7 @@
         <v>1685</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>48</v>
@@ -8065,7 +8059,7 @@
         <v>1685</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>51</v>
@@ -8100,7 +8094,7 @@
         <v>1685</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>54</v>
@@ -8135,7 +8129,7 @@
         <v>1685</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>57</v>
@@ -8170,7 +8164,7 @@
         <v>1685</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>60</v>
@@ -8205,7 +8199,7 @@
         <v>63</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>64</v>
@@ -8240,7 +8234,7 @@
         <v>63</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>68</v>
@@ -8275,7 +8269,7 @@
         <v>71</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>72</v>
@@ -8310,7 +8304,7 @@
         <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>76</v>
@@ -8342,10 +8336,10 @@
         <v>2012</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>2043</v>
+        <v>2039</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>79</v>
@@ -8377,10 +8371,10 @@
         <v>2012</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>2043</v>
+        <v>2039</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>82</v>
@@ -8412,10 +8406,10 @@
         <v>2012</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>2044</v>
+        <v>2040</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>85</v>
@@ -8447,10 +8441,10 @@
         <v>2012</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>2044</v>
+        <v>2040</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>88</v>
@@ -8482,10 +8476,10 @@
         <v>2012</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>91</v>
@@ -8517,10 +8511,10 @@
         <v>2012</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>93</v>
@@ -8552,10 +8546,10 @@
         <v>2012</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>2042</v>
+        <v>1614</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>2044</v>
+        <v>2040</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>96</v>
@@ -8590,7 +8584,7 @@
         <v>99</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>100</v>
@@ -8657,10 +8651,10 @@
         <v>2012</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>110</v>
@@ -8765,7 +8759,7 @@
         <v>1685</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>2045</v>
+        <v>2041</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>121</v>
@@ -8800,7 +8794,7 @@
         <v>1685</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>2046</v>
+        <v>2042</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>124</v>
@@ -8835,7 +8829,7 @@
         <v>1685</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>127</v>
@@ -8870,7 +8864,7 @@
         <v>1685</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>2047</v>
+        <v>2043</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>130</v>
@@ -8905,7 +8899,7 @@
         <v>1685</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>2048</v>
+        <v>2044</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>133</v>
@@ -8975,7 +8969,7 @@
         <v>1685</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>2049</v>
+        <v>2045</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>140</v>
@@ -9010,7 +9004,7 @@
         <v>1685</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>2050</v>
+        <v>2046</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>143</v>
@@ -9045,7 +9039,7 @@
         <v>1685</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>2051</v>
+        <v>2047</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>146</v>
@@ -9115,7 +9109,7 @@
         <v>1685</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>153</v>
@@ -9150,7 +9144,7 @@
         <v>1685</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>2052</v>
+        <v>2048</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>156</v>
@@ -9185,7 +9179,7 @@
         <v>1685</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>2053</v>
+        <v>2049</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>159</v>
@@ -9288,7 +9282,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>173</v>
@@ -9323,7 +9317,7 @@
         <v>10</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>2054</v>
+        <v>2050</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>176</v>
@@ -9358,7 +9352,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>2054</v>
+        <v>2050</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>179</v>
@@ -9393,7 +9387,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>182</v>
@@ -9434,7 +9428,7 @@
         <v>186</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>2221</v>
+        <v>2215</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>19</v>
@@ -9463,7 +9457,7 @@
         <v>1785</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>188</v>
@@ -9568,7 +9562,7 @@
         <v>1614</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>197</v>
@@ -9603,7 +9597,7 @@
         <v>1614</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>200</v>
@@ -9638,7 +9632,7 @@
         <v>1609</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>2055</v>
+        <v>2051</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>203</v>
@@ -9673,7 +9667,7 @@
         <v>1610</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>206</v>
@@ -9708,7 +9702,7 @@
         <v>1610</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>209</v>
@@ -9743,7 +9737,7 @@
         <v>1685</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>212</v>
@@ -9813,7 +9807,7 @@
         <v>1685</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>219</v>
@@ -9848,13 +9842,13 @@
         <v>10</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>2104</v>
+        <v>2100</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>222</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>19</v>
@@ -9883,7 +9877,7 @@
         <v>10</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>224</v>
@@ -9918,13 +9912,13 @@
         <v>10</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>2106</v>
+        <v>2102</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>227</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>2190</v>
+        <v>2184</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>13</v>
@@ -9953,7 +9947,7 @@
         <v>10</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>229</v>
@@ -9988,13 +9982,13 @@
         <v>10</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>2107</v>
+        <v>2103</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>232</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>19</v>
@@ -10023,7 +10017,7 @@
         <v>10</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>2108</v>
+        <v>2104</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>234</v>
@@ -10058,7 +10052,7 @@
         <v>10</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>2109</v>
+        <v>2105</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>237</v>
@@ -10093,7 +10087,7 @@
         <v>1785</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>241</v>
@@ -10128,7 +10122,7 @@
         <v>1785</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>245</v>
@@ -10163,7 +10157,7 @@
         <v>1785</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>249</v>
@@ -10198,7 +10192,7 @@
         <v>1785</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>253</v>
@@ -10233,7 +10227,7 @@
         <v>1785</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>257</v>
@@ -10268,7 +10262,7 @@
         <v>1785</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>261</v>
@@ -10303,7 +10297,7 @@
         <v>1785</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>265</v>
@@ -10338,7 +10332,7 @@
         <v>1785</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>268</v>
@@ -10408,7 +10402,7 @@
         <v>1609</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>2110</v>
+        <v>2106</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>275</v>
@@ -10443,7 +10437,7 @@
         <v>1609</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>2111</v>
+        <v>2107</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>278</v>
@@ -10478,7 +10472,7 @@
         <v>1609</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>2112</v>
+        <v>2108</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>281</v>
@@ -10513,7 +10507,7 @@
         <v>1609</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>284</v>
@@ -10548,7 +10542,7 @@
         <v>1609</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>287</v>
@@ -10583,7 +10577,7 @@
         <v>1609</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>2114</v>
+        <v>2110</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>290</v>
@@ -10618,7 +10612,7 @@
         <v>1609</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>2111</v>
+        <v>2107</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>293</v>
@@ -10653,7 +10647,7 @@
         <v>1609</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>2115</v>
+        <v>2111</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>296</v>
@@ -10688,7 +10682,7 @@
         <v>1609</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>2116</v>
+        <v>2112</v>
       </c>
       <c r="E89" s="4" t="s">
         <v>299</v>
@@ -10723,7 +10717,7 @@
         <v>1609</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>2117</v>
+        <v>2113</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>302</v>
@@ -10758,7 +10752,7 @@
         <v>1609</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>2117</v>
+        <v>2113</v>
       </c>
       <c r="E91" s="4" t="s">
         <v>305</v>
@@ -10793,7 +10787,7 @@
         <v>1609</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>2118</v>
+        <v>2114</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>308</v>
@@ -10828,7 +10822,7 @@
         <v>1610</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="E93" s="4" t="s">
         <v>311</v>
@@ -10863,7 +10857,7 @@
         <v>1610</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>2119</v>
+        <v>2115</v>
       </c>
       <c r="E94" s="4" t="s">
         <v>314</v>
@@ -10898,7 +10892,7 @@
         <v>1610</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>317</v>
@@ -10933,13 +10927,13 @@
         <v>1610</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>2118</v>
+        <v>2114</v>
       </c>
       <c r="E96" s="4" t="s">
         <v>320</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>19</v>
@@ -10968,7 +10962,7 @@
         <v>1610</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>322</v>
@@ -11003,7 +10997,7 @@
         <v>1610</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>2121</v>
+        <v>2117</v>
       </c>
       <c r="E98" s="4" t="s">
         <v>325</v>
@@ -11038,7 +11032,7 @@
         <v>1610</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>328</v>
@@ -11073,7 +11067,7 @@
         <v>1610</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>331</v>
@@ -11108,7 +11102,7 @@
         <v>1789</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>2122</v>
+        <v>2118</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>334</v>
@@ -11143,7 +11137,7 @@
         <v>10</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>2123</v>
+        <v>2119</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>338</v>
@@ -11178,7 +11172,7 @@
         <v>10</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>341</v>
@@ -11213,7 +11207,7 @@
         <v>10</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>2122</v>
+        <v>2118</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>345</v>
@@ -11248,7 +11242,7 @@
         <v>1785</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>349</v>
@@ -11283,7 +11277,7 @@
         <v>1785</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>353</v>
@@ -11318,7 +11312,7 @@
         <v>1785</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>357</v>
@@ -11353,7 +11347,7 @@
         <v>1785</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>360</v>
@@ -11388,7 +11382,7 @@
         <v>1785</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>364</v>
@@ -11423,7 +11417,7 @@
         <v>1785</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>368</v>
@@ -11458,7 +11452,7 @@
         <v>1785</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>372</v>
@@ -11493,7 +11487,7 @@
         <v>1785</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>376</v>
@@ -11528,7 +11522,7 @@
         <v>1614</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>379</v>
@@ -11563,7 +11557,7 @@
         <v>382</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>2120</v>
+        <v>2116</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>383</v>
@@ -11598,7 +11592,7 @@
         <v>382</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>387</v>
@@ -11633,7 +11627,7 @@
         <v>1609</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>391</v>
@@ -11668,7 +11662,7 @@
         <v>1609</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>395</v>
@@ -11703,7 +11697,7 @@
         <v>1609</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="E118" s="4" t="s">
         <v>399</v>
@@ -11738,7 +11732,7 @@
         <v>1609</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>402</v>
@@ -11773,7 +11767,7 @@
         <v>1609</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>2124</v>
+        <v>2120</v>
       </c>
       <c r="E120" s="4" t="s">
         <v>405</v>
@@ -11808,7 +11802,7 @@
         <v>1610</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>2125</v>
+        <v>2121</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>408</v>
@@ -11843,7 +11837,7 @@
         <v>1610</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="E122" t="s">
         <v>1553</v>
@@ -11878,7 +11872,7 @@
         <v>1610</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>2056</v>
+        <v>2052</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>415</v>
@@ -11913,7 +11907,7 @@
         <v>1610</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>2057</v>
+        <v>2053</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>418</v>
@@ -11948,7 +11942,7 @@
         <v>1610</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>2057</v>
+        <v>2053</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>421</v>
@@ -11983,7 +11977,7 @@
         <v>1610</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>2126</v>
+        <v>2122</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>424</v>
@@ -12018,7 +12012,7 @@
         <v>1610</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>2125</v>
+        <v>2121</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>428</v>
@@ -12053,7 +12047,7 @@
         <v>1627</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>2058</v>
+        <v>2054</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>431</v>
@@ -12088,7 +12082,7 @@
         <v>1789</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>2127</v>
+        <v>2123</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>434</v>
@@ -12123,13 +12117,13 @@
         <v>1789</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>2059</v>
+        <v>2055</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>438</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>2191</v>
+        <v>2185</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>13</v>
@@ -12158,7 +12152,7 @@
         <v>1789</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>2128</v>
+        <v>2124</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>441</v>
@@ -12193,7 +12187,7 @@
         <v>1789</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>2128</v>
+        <v>2124</v>
       </c>
       <c r="E132" s="4" t="s">
         <v>445</v>
@@ -12228,7 +12222,7 @@
         <v>10</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>2060</v>
+        <v>2056</v>
       </c>
       <c r="E133" s="4" t="s">
         <v>449</v>
@@ -12263,7 +12257,7 @@
         <v>10</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>2061</v>
+        <v>2057</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>452</v>
@@ -12298,7 +12292,7 @@
         <v>10</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>2062</v>
+        <v>2058</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>455</v>
@@ -12333,7 +12327,7 @@
         <v>1785</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>2063</v>
+        <v>2059</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>458</v>
@@ -12368,7 +12362,7 @@
         <v>1614</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>461</v>
@@ -12403,7 +12397,7 @@
         <v>1614</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>465</v>
@@ -12438,7 +12432,7 @@
         <v>1614</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>2109</v>
+        <v>2105</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>469</v>
@@ -12473,7 +12467,7 @@
         <v>382</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>2064</v>
+        <v>2060</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>472</v>
@@ -12508,7 +12502,7 @@
         <v>382</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>2065</v>
+        <v>2061</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>475</v>
@@ -12543,7 +12537,7 @@
         <v>1609</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>2066</v>
+        <v>2062</v>
       </c>
       <c r="E142" s="4" t="s">
         <v>479</v>
@@ -12578,7 +12572,7 @@
         <v>1610</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>2067</v>
+        <v>2063</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>483</v>
@@ -12613,7 +12607,7 @@
         <v>487</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>2142</v>
+        <v>2138</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>488</v>
@@ -12648,7 +12642,7 @@
         <v>1627</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>2143</v>
+        <v>2139</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>491</v>
@@ -12683,7 +12677,7 @@
         <v>1627</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>2068</v>
+        <v>2064</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>494</v>
@@ -12718,7 +12712,7 @@
         <v>1627</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>498</v>
@@ -12753,7 +12747,7 @@
         <v>1627</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>501</v>
@@ -12788,7 +12782,7 @@
         <v>1631</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="E149" s="4" t="s">
         <v>504</v>
@@ -12823,7 +12817,7 @@
         <v>10</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>2145</v>
+        <v>2141</v>
       </c>
       <c r="E150" s="4" t="s">
         <v>507</v>
@@ -12858,7 +12852,7 @@
         <v>10</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>2069</v>
+        <v>2065</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>510</v>
@@ -12893,13 +12887,13 @@
         <v>10</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>2146</v>
+        <v>2142</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>513</v>
       </c>
       <c r="F152" s="4" t="s">
-        <v>2147</v>
+        <v>2143</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>19</v>
@@ -12928,7 +12922,7 @@
         <v>10</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>2148</v>
+        <v>2144</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>515</v>
@@ -12963,7 +12957,7 @@
         <v>10</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>2149</v>
+        <v>2145</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>518</v>
@@ -12998,7 +12992,7 @@
         <v>10</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>2150</v>
+        <v>2146</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>521</v>
@@ -13033,7 +13027,7 @@
         <v>10</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>2150</v>
+        <v>2146</v>
       </c>
       <c r="E156" s="4" t="s">
         <v>524</v>
@@ -13103,7 +13097,7 @@
         <v>10</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>2070</v>
+        <v>2066</v>
       </c>
       <c r="E158" s="4" t="s">
         <v>532</v>
@@ -13138,7 +13132,7 @@
         <v>536</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>2071</v>
+        <v>2067</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>537</v>
@@ -13173,7 +13167,7 @@
         <v>536</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>2072</v>
+        <v>2068</v>
       </c>
       <c r="E160" s="4" t="s">
         <v>540</v>
@@ -13208,7 +13202,7 @@
         <v>536</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>543</v>
@@ -13243,7 +13237,7 @@
         <v>536</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>2073</v>
+        <v>2069</v>
       </c>
       <c r="E162" s="4" t="s">
         <v>546</v>
@@ -13278,7 +13272,7 @@
         <v>550</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>551</v>
@@ -13313,7 +13307,7 @@
         <v>550</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="E164" s="4" t="s">
         <v>555</v>
@@ -13348,7 +13342,7 @@
         <v>550</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>2074</v>
+        <v>2070</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>559</v>
@@ -13383,7 +13377,7 @@
         <v>550</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>2072</v>
+        <v>2068</v>
       </c>
       <c r="E166" s="4" t="s">
         <v>562</v>
@@ -13418,7 +13412,7 @@
         <v>550</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>2075</v>
+        <v>2071</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>565</v>
@@ -13453,7 +13447,7 @@
         <v>1614</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>2151</v>
+        <v>2147</v>
       </c>
       <c r="E168" s="4" t="s">
         <v>568</v>
@@ -13488,7 +13482,7 @@
         <v>1614</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>572</v>
@@ -13558,7 +13552,7 @@
         <v>580</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>2152</v>
+        <v>2148</v>
       </c>
       <c r="E171" s="4" t="s">
         <v>581</v>
@@ -13593,7 +13587,7 @@
         <v>580</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>2076</v>
+        <v>2072</v>
       </c>
       <c r="E172" s="4" t="s">
         <v>585</v>
@@ -13628,7 +13622,7 @@
         <v>580</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>2153</v>
+        <v>2149</v>
       </c>
       <c r="E173" s="4" t="s">
         <v>589</v>
@@ -13663,13 +13657,13 @@
         <v>580</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>2077</v>
+        <v>2073</v>
       </c>
       <c r="E174" s="4" t="s">
         <v>592</v>
       </c>
       <c r="F174" s="4" t="s">
-        <v>2192</v>
+        <v>2186</v>
       </c>
       <c r="G174" s="1" t="s">
         <v>13</v>
@@ -13698,7 +13692,7 @@
         <v>580</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>2152</v>
+        <v>2148</v>
       </c>
       <c r="E175" s="4" t="s">
         <v>581</v>
@@ -13733,7 +13727,7 @@
         <v>382</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>2154</v>
+        <v>2150</v>
       </c>
       <c r="E176" s="4" t="s">
         <v>596</v>
@@ -13768,7 +13762,7 @@
         <v>382</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>2155</v>
+        <v>2151</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>599</v>
@@ -13803,7 +13797,7 @@
         <v>382</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>2156</v>
+        <v>2152</v>
       </c>
       <c r="E178" s="4" t="s">
         <v>602</v>
@@ -13838,7 +13832,7 @@
         <v>606</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>2078</v>
+        <v>2074</v>
       </c>
       <c r="E179" s="4" t="s">
         <v>607</v>
@@ -13873,7 +13867,7 @@
         <v>606</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>2157</v>
+        <v>2153</v>
       </c>
       <c r="E180" s="4" t="s">
         <v>611</v>
@@ -13908,7 +13902,7 @@
         <v>606</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>2079</v>
+        <v>2075</v>
       </c>
       <c r="E181" s="4" t="s">
         <v>615</v>
@@ -13943,7 +13937,7 @@
         <v>1640</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="E182" s="4" t="s">
         <v>619</v>
@@ -13978,7 +13972,7 @@
         <v>1640</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>2158</v>
+        <v>2154</v>
       </c>
       <c r="E183" s="4" t="s">
         <v>622</v>
@@ -14013,7 +14007,7 @@
         <v>1640</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="E184" s="4" t="s">
         <v>625</v>
@@ -14048,7 +14042,7 @@
         <v>1640</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>2159</v>
+        <v>2155</v>
       </c>
       <c r="E185" s="4" t="s">
         <v>629</v>
@@ -14083,7 +14077,7 @@
         <v>1685</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>2080</v>
+        <v>2076</v>
       </c>
       <c r="E186" s="4" t="s">
         <v>632</v>
@@ -14118,7 +14112,7 @@
         <v>1685</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>2160</v>
+        <v>2156</v>
       </c>
       <c r="E187" s="4" t="s">
         <v>635</v>
@@ -14153,7 +14147,7 @@
         <v>1627</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="E188" s="4" t="s">
         <v>639</v>
@@ -14188,7 +14182,7 @@
         <v>1627</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>2081</v>
+        <v>2077</v>
       </c>
       <c r="E189" s="4" t="s">
         <v>642</v>
@@ -14223,7 +14217,7 @@
         <v>1627</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>2082</v>
+        <v>2078</v>
       </c>
       <c r="E190" s="4" t="s">
         <v>646</v>
@@ -14258,13 +14252,13 @@
         <v>1627</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="E191" s="4" t="s">
         <v>649</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="G191" s="1" t="s">
         <v>19</v>
@@ -14293,7 +14287,7 @@
         <v>1615</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>2083</v>
+        <v>2079</v>
       </c>
       <c r="E192" s="4" t="s">
         <v>652</v>
@@ -14328,7 +14322,7 @@
         <v>1615</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>2161</v>
+        <v>2157</v>
       </c>
       <c r="E193" s="4" t="s">
         <v>655</v>
@@ -14360,10 +14354,10 @@
         <v>2018</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>2197</v>
+        <v>2191</v>
       </c>
       <c r="E194" s="4" t="s">
         <v>658</v>
@@ -14395,10 +14389,10 @@
         <v>2018</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>2198</v>
+        <v>2192</v>
       </c>
       <c r="E195" s="4" t="s">
         <v>661</v>
@@ -14430,10 +14424,10 @@
         <v>2018</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>2199</v>
+        <v>2193</v>
       </c>
       <c r="E196" s="4" t="s">
         <v>664</v>
@@ -14465,10 +14459,10 @@
         <v>2018</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>2197</v>
+        <v>2191</v>
       </c>
       <c r="E197" s="4" t="s">
         <v>668</v>
@@ -14503,7 +14497,7 @@
         <v>1631</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>2200</v>
+        <v>2194</v>
       </c>
       <c r="E198" s="4" t="s">
         <v>671</v>
@@ -14538,7 +14532,7 @@
         <v>1631</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="E199" s="4" t="s">
         <v>674</v>
@@ -14573,7 +14567,7 @@
         <v>1631</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E200" s="4" t="s">
         <v>677</v>
@@ -14608,7 +14602,7 @@
         <v>550</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="E201" s="4" t="s">
         <v>680</v>
@@ -14643,7 +14637,7 @@
         <v>550</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>2144</v>
+        <v>2140</v>
       </c>
       <c r="E202" s="4" t="s">
         <v>683</v>
@@ -14678,7 +14672,7 @@
         <v>550</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="E203" s="4" t="s">
         <v>686</v>
@@ -14713,7 +14707,7 @@
         <v>550</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>2201</v>
+        <v>2195</v>
       </c>
       <c r="E204" s="4" t="s">
         <v>690</v>
@@ -14748,7 +14742,7 @@
         <v>1614</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>2162</v>
+        <v>2158</v>
       </c>
       <c r="E205" s="4" t="s">
         <v>694</v>
@@ -14783,7 +14777,7 @@
         <v>1614</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="E206" s="4" t="s">
         <v>697</v>
@@ -14818,7 +14812,7 @@
         <v>1614</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="E207" s="4" t="s">
         <v>700</v>
@@ -14853,7 +14847,7 @@
         <v>1614</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>2202</v>
+        <v>2196</v>
       </c>
       <c r="E208" s="4" t="s">
         <v>703</v>
@@ -14888,7 +14882,7 @@
         <v>1614</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>2203</v>
+        <v>2197</v>
       </c>
       <c r="E209" s="4" t="s">
         <v>706</v>
@@ -14923,7 +14917,7 @@
         <v>580</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="E210" s="4" t="s">
         <v>710</v>
@@ -14958,7 +14952,7 @@
         <v>580</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>2084</v>
+        <v>2080</v>
       </c>
       <c r="E211" s="4" t="s">
         <v>714</v>
@@ -14993,7 +14987,7 @@
         <v>580</v>
       </c>
       <c r="D212" s="4" t="s">
-        <v>2085</v>
+        <v>2081</v>
       </c>
       <c r="E212" s="4" t="s">
         <v>718</v>
@@ -15028,7 +15022,7 @@
         <v>580</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>2163</v>
+        <v>2159</v>
       </c>
       <c r="E213" s="4" t="s">
         <v>722</v>
@@ -15063,7 +15057,7 @@
         <v>1624</v>
       </c>
       <c r="D214" s="4" t="s">
-        <v>2084</v>
+        <v>2080</v>
       </c>
       <c r="E214" s="4" t="s">
         <v>726</v>
@@ -15098,7 +15092,7 @@
         <v>1624</v>
       </c>
       <c r="D215" s="4" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="E215" s="4" t="s">
         <v>729</v>
@@ -15133,7 +15127,7 @@
         <v>1624</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>2164</v>
+        <v>2160</v>
       </c>
       <c r="E216" s="4" t="s">
         <v>732</v>
@@ -15168,7 +15162,7 @@
         <v>1624</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="E217" s="4" t="s">
         <v>736</v>
@@ -15203,7 +15197,7 @@
         <v>1620</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>2165</v>
+        <v>2161</v>
       </c>
       <c r="E218" s="4" t="s">
         <v>740</v>
@@ -15238,7 +15232,7 @@
         <v>1620</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>2166</v>
+        <v>2162</v>
       </c>
       <c r="E219" s="4" t="s">
         <v>743</v>
@@ -15273,7 +15267,7 @@
         <v>1620</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>2167</v>
+        <v>2163</v>
       </c>
       <c r="E220" s="4" t="s">
         <v>746</v>
@@ -15308,7 +15302,7 @@
         <v>1616</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>2086</v>
+        <v>2082</v>
       </c>
       <c r="E221" s="4" t="s">
         <v>749</v>
@@ -15343,7 +15337,7 @@
         <v>1616</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>2197</v>
+        <v>2191</v>
       </c>
       <c r="E222" s="4" t="s">
         <v>753</v>
@@ -15378,7 +15372,7 @@
         <v>1616</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="E223" s="4" t="s">
         <v>757</v>
@@ -15413,7 +15407,7 @@
         <v>1685</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>2087</v>
+        <v>2083</v>
       </c>
       <c r="E224" s="4" t="s">
         <v>761</v>
@@ -15448,7 +15442,7 @@
         <v>1685</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="E225" s="4" t="s">
         <v>764</v>
@@ -15518,7 +15512,7 @@
         <v>1685</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="E227" s="4" t="s">
         <v>771</v>
@@ -15553,7 +15547,7 @@
         <v>1685</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>2088</v>
+        <v>2084</v>
       </c>
       <c r="E228" s="4" t="s">
         <v>775</v>
@@ -15588,7 +15582,7 @@
         <v>1685</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>2204</v>
+        <v>2198</v>
       </c>
       <c r="E229" s="4" t="s">
         <v>778</v>
@@ -15623,7 +15617,7 @@
         <v>1640</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>2086</v>
+        <v>2082</v>
       </c>
       <c r="E230" s="4" t="s">
         <v>781</v>
@@ -15658,7 +15652,7 @@
         <v>1640</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="E231" s="4" t="s">
         <v>784</v>
@@ -15693,7 +15687,7 @@
         <v>1640</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>2089</v>
+        <v>2085</v>
       </c>
       <c r="E232" s="4" t="s">
         <v>788</v>
@@ -15728,7 +15722,7 @@
         <v>1640</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>2090</v>
+        <v>2086</v>
       </c>
       <c r="E233" s="4" t="s">
         <v>791</v>
@@ -15763,7 +15757,7 @@
         <v>1627</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>2091</v>
+        <v>2087</v>
       </c>
       <c r="E234" s="4" t="s">
         <v>795</v>
@@ -15798,7 +15792,7 @@
         <v>1627</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>2092</v>
+        <v>2088</v>
       </c>
       <c r="E235" s="4" t="s">
         <v>798</v>
@@ -15833,7 +15827,7 @@
         <v>1627</v>
       </c>
       <c r="D236" s="4" t="s">
-        <v>2092</v>
+        <v>2088</v>
       </c>
       <c r="E236" s="4" t="s">
         <v>801</v>
@@ -15868,7 +15862,7 @@
         <v>1627</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>2093</v>
+        <v>2089</v>
       </c>
       <c r="E237" s="4" t="s">
         <v>804</v>
@@ -15903,7 +15897,7 @@
         <v>1627</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>2092</v>
+        <v>2088</v>
       </c>
       <c r="E238" s="4" t="s">
         <v>808</v>
@@ -15938,7 +15932,7 @@
         <v>1615</v>
       </c>
       <c r="D239" s="4" t="s">
-        <v>2094</v>
+        <v>2090</v>
       </c>
       <c r="E239" s="4" t="s">
         <v>811</v>
@@ -15973,7 +15967,7 @@
         <v>1615</v>
       </c>
       <c r="D240" s="4" t="s">
-        <v>2168</v>
+        <v>2164</v>
       </c>
       <c r="E240" s="4" t="s">
         <v>814</v>
@@ -16008,7 +16002,7 @@
         <v>1615</v>
       </c>
       <c r="D241" s="4" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E241" s="4" t="s">
         <v>817</v>
@@ -16043,7 +16037,7 @@
         <v>1615</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>2095</v>
+        <v>2091</v>
       </c>
       <c r="E242" s="4" t="s">
         <v>820</v>
@@ -16078,7 +16072,7 @@
         <v>1615</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>2169</v>
+        <v>2165</v>
       </c>
       <c r="E243" s="4" t="s">
         <v>823</v>
@@ -16113,7 +16107,7 @@
         <v>1615</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="E244" s="4" t="s">
         <v>826</v>
@@ -16145,10 +16139,10 @@
         <v>2019</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>2170</v>
+        <v>2166</v>
       </c>
       <c r="E245" s="4" t="s">
         <v>829</v>
@@ -16180,10 +16174,10 @@
         <v>2019</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>2171</v>
+        <v>2167</v>
       </c>
       <c r="E246" s="4" t="s">
         <v>832</v>
@@ -16215,10 +16209,10 @@
         <v>2019</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D247" s="4" t="s">
-        <v>2096</v>
+        <v>2092</v>
       </c>
       <c r="E247" s="4" t="s">
         <v>835</v>
@@ -16250,7 +16244,7 @@
         <v>2019</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>838</v>
@@ -16285,10 +16279,10 @@
         <v>2019</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D249" s="4" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="E249" s="4" t="s">
         <v>842</v>
@@ -16323,7 +16317,7 @@
         <v>1631</v>
       </c>
       <c r="D250" s="4" t="s">
-        <v>2205</v>
+        <v>2199</v>
       </c>
       <c r="E250" s="4" t="s">
         <v>845</v>
@@ -16358,7 +16352,7 @@
         <v>1631</v>
       </c>
       <c r="D251" s="4" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="E251" s="4" t="s">
         <v>848</v>
@@ -16393,7 +16387,7 @@
         <v>550</v>
       </c>
       <c r="D252" s="4" t="s">
-        <v>2097</v>
+        <v>2093</v>
       </c>
       <c r="E252" s="4" t="s">
         <v>851</v>
@@ -16428,7 +16422,7 @@
         <v>550</v>
       </c>
       <c r="D253" s="4" t="s">
-        <v>2098</v>
+        <v>2094</v>
       </c>
       <c r="E253" s="4" t="s">
         <v>854</v>
@@ -16463,7 +16457,7 @@
         <v>550</v>
       </c>
       <c r="D254" s="4" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="E254" s="4" t="s">
         <v>857</v>
@@ -16498,13 +16492,13 @@
         <v>550</v>
       </c>
       <c r="D255" s="4" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="E255" s="4" t="s">
         <v>860</v>
       </c>
       <c r="F255" s="4" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="G255" s="4" t="s">
         <v>13</v>
@@ -16533,7 +16527,7 @@
         <v>550</v>
       </c>
       <c r="D256" s="4" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="E256" s="4" t="s">
         <v>862</v>
@@ -16568,7 +16562,7 @@
         <v>580</v>
       </c>
       <c r="D257" s="4" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="E257" s="4" t="s">
         <v>865</v>
@@ -16603,7 +16597,7 @@
         <v>580</v>
       </c>
       <c r="D258" s="4" t="s">
-        <v>2206</v>
+        <v>2200</v>
       </c>
       <c r="E258" s="4" t="s">
         <v>869</v>
@@ -16638,7 +16632,7 @@
         <v>580</v>
       </c>
       <c r="D259" s="4" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="E259" s="4" t="s">
         <v>872</v>
@@ -16673,7 +16667,7 @@
         <v>580</v>
       </c>
       <c r="D260" s="4" t="s">
-        <v>2099</v>
+        <v>2095</v>
       </c>
       <c r="E260" s="4" t="s">
         <v>876</v>
@@ -16708,13 +16702,13 @@
         <v>580</v>
       </c>
       <c r="D261" s="4" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="E261" s="4" t="s">
         <v>879</v>
       </c>
       <c r="F261" s="4" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="G261" s="4" t="s">
         <v>13</v>
@@ -16743,7 +16737,7 @@
         <v>1614</v>
       </c>
       <c r="D262" s="4" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="E262" s="4" t="s">
         <v>882</v>
@@ -16778,7 +16772,7 @@
         <v>1614</v>
       </c>
       <c r="D263" s="4" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="E263" s="4" t="s">
         <v>885</v>
@@ -16813,7 +16807,7 @@
         <v>1614</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="E264" s="4" t="s">
         <v>888</v>
@@ -16848,7 +16842,7 @@
         <v>1614</v>
       </c>
       <c r="D265" s="4" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="E265" s="4" t="s">
         <v>891</v>
@@ -16883,7 +16877,7 @@
         <v>1614</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="E266" s="4" t="s">
         <v>894</v>
@@ -16918,7 +16912,7 @@
         <v>1614</v>
       </c>
       <c r="D267" s="4" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="E267" s="4" t="s">
         <v>897</v>
@@ -16953,7 +16947,7 @@
         <v>1624</v>
       </c>
       <c r="D268" s="4" t="s">
-        <v>2207</v>
+        <v>2201</v>
       </c>
       <c r="E268" s="4" t="s">
         <v>900</v>
@@ -16988,7 +16982,7 @@
         <v>1624</v>
       </c>
       <c r="D269" s="4" t="s">
-        <v>2207</v>
+        <v>2201</v>
       </c>
       <c r="E269" s="4" t="s">
         <v>903</v>
@@ -17023,7 +17017,7 @@
         <v>1624</v>
       </c>
       <c r="D270" s="4" t="s">
-        <v>2207</v>
+        <v>2201</v>
       </c>
       <c r="E270" s="4" t="s">
         <v>907</v>
@@ -17058,7 +17052,7 @@
         <v>1624</v>
       </c>
       <c r="D271" s="4" t="s">
-        <v>2207</v>
+        <v>2201</v>
       </c>
       <c r="E271" s="4" t="s">
         <v>911</v>
@@ -17093,7 +17087,7 @@
         <v>1620</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="E272" s="4" t="s">
         <v>914</v>
@@ -17128,7 +17122,7 @@
         <v>1620</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>2172</v>
+        <v>2168</v>
       </c>
       <c r="E273" s="4" t="s">
         <v>917</v>
@@ -17140,7 +17134,7 @@
         <v>19</v>
       </c>
       <c r="H273" s="10" t="s">
-        <v>2208</v>
+        <v>2202</v>
       </c>
       <c r="I273" s="4" t="s">
         <v>15</v>
@@ -17163,7 +17157,7 @@
         <v>1620</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="E274" s="4" t="s">
         <v>919</v>
@@ -17198,7 +17192,7 @@
         <v>1620</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>2174</v>
+        <v>2170</v>
       </c>
       <c r="E275" s="4" t="s">
         <v>922</v>
@@ -17233,7 +17227,7 @@
         <v>1620</v>
       </c>
       <c r="D276" s="4" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
       <c r="E276" s="4" t="s">
         <v>925</v>
@@ -17268,7 +17262,7 @@
         <v>1620</v>
       </c>
       <c r="D277" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
       <c r="E277" s="4" t="s">
         <v>929</v>
@@ -17303,7 +17297,7 @@
         <v>1620</v>
       </c>
       <c r="D278" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
       <c r="E278" s="4" t="s">
         <v>932</v>
@@ -17338,7 +17332,7 @@
         <v>1616</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>2209</v>
+        <v>2203</v>
       </c>
       <c r="E279" s="4" t="s">
         <v>936</v>
@@ -17373,7 +17367,7 @@
         <v>1616</v>
       </c>
       <c r="D280" s="4" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="E280" s="4" t="s">
         <v>939</v>
@@ -17385,7 +17379,7 @@
         <v>19</v>
       </c>
       <c r="H280" s="11" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="I280" s="4" t="s">
         <v>15</v>
@@ -17408,7 +17402,7 @@
         <v>1616</v>
       </c>
       <c r="D281" s="4" t="s">
-        <v>2210</v>
+        <v>2204</v>
       </c>
       <c r="E281" s="4" t="s">
         <v>941</v>
@@ -17443,7 +17437,7 @@
         <v>1616</v>
       </c>
       <c r="D282" s="4" t="s">
-        <v>2173</v>
+        <v>2169</v>
       </c>
       <c r="E282" s="4" t="s">
         <v>944</v>
@@ -17478,7 +17472,7 @@
         <v>1616</v>
       </c>
       <c r="D283" s="4" t="s">
-        <v>2175</v>
+        <v>2171</v>
       </c>
       <c r="E283" s="4" t="s">
         <v>947</v>
@@ -17513,7 +17507,7 @@
         <v>1616</v>
       </c>
       <c r="D284" s="4" t="s">
-        <v>2211</v>
+        <v>2205</v>
       </c>
       <c r="E284" s="4" t="s">
         <v>950</v>
@@ -17548,7 +17542,7 @@
         <v>1616</v>
       </c>
       <c r="D285" s="4" t="s">
-        <v>2212</v>
+        <v>2206</v>
       </c>
       <c r="E285" s="4" t="s">
         <v>953</v>
@@ -17583,7 +17577,7 @@
         <v>1640</v>
       </c>
       <c r="D286" s="4" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
       <c r="E286" s="4" t="s">
         <v>957</v>
@@ -17618,7 +17612,7 @@
         <v>1640</v>
       </c>
       <c r="D287" s="4" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
       <c r="E287" s="4" t="s">
         <v>961</v>
@@ -17653,7 +17647,7 @@
         <v>1640</v>
       </c>
       <c r="D288" s="4" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
       <c r="E288" s="4" t="s">
         <v>965</v>
@@ -17688,7 +17682,7 @@
         <v>1640</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
       <c r="E289" s="4" t="s">
         <v>968</v>
@@ -17723,7 +17717,7 @@
         <v>1640</v>
       </c>
       <c r="D290" s="4" t="s">
-        <v>2103</v>
+        <v>2099</v>
       </c>
       <c r="E290" s="4" t="s">
         <v>972</v>
@@ -17758,7 +17752,7 @@
         <v>1640</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="E291" s="4" t="s">
         <v>975</v>
@@ -17790,7 +17784,7 @@
         <v>2021</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D292" s="4" t="s">
         <v>1907</v>
@@ -17825,10 +17819,10 @@
         <v>2021</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D293" s="4" t="s">
-        <v>2176</v>
+        <v>2227</v>
       </c>
       <c r="E293" s="4" t="s">
         <v>981</v>
@@ -17863,7 +17857,7 @@
         <v>1631</v>
       </c>
       <c r="D294" s="4" t="s">
-        <v>2033</v>
+        <v>2228</v>
       </c>
       <c r="E294" s="4" t="s">
         <v>984</v>
@@ -17898,7 +17892,7 @@
         <v>987</v>
       </c>
       <c r="D295" s="4" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="E295" s="4" t="s">
         <v>988</v>
@@ -17930,7 +17924,7 @@
         <v>2022</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D296" s="4" t="s">
         <v>1908</v>
@@ -17939,7 +17933,7 @@
         <v>992</v>
       </c>
       <c r="F296" s="4" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="G296" s="1" t="s">
         <v>66</v>
@@ -17965,7 +17959,7 @@
         <v>1631</v>
       </c>
       <c r="D297" s="4" t="s">
-        <v>2034</v>
+        <v>2229</v>
       </c>
       <c r="E297" s="4" t="s">
         <v>993</v>
@@ -18000,7 +17994,7 @@
         <v>1785</v>
       </c>
       <c r="D298" s="4" t="s">
-        <v>2222</v>
+        <v>2216</v>
       </c>
       <c r="E298" s="4" t="s">
         <v>996</v>
@@ -18035,7 +18029,7 @@
         <v>1785</v>
       </c>
       <c r="D299" s="4" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="E299" s="4" t="s">
         <v>999</v>
@@ -18070,7 +18064,7 @@
         <v>1785</v>
       </c>
       <c r="D300" s="4" t="s">
-        <v>2223</v>
+        <v>2217</v>
       </c>
       <c r="E300" s="4" t="s">
         <v>1003</v>
@@ -18105,7 +18099,7 @@
         <v>580</v>
       </c>
       <c r="D301" s="4" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="E301" s="4" t="s">
         <v>1006</v>
@@ -18140,7 +18134,7 @@
         <v>580</v>
       </c>
       <c r="D302" s="4" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="E302" s="4" t="s">
         <v>1009</v>
@@ -18175,7 +18169,7 @@
         <v>1624</v>
       </c>
       <c r="D303" s="4" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="E303" s="4" t="s">
         <v>1012</v>
@@ -18210,7 +18204,7 @@
         <v>1624</v>
       </c>
       <c r="D304" s="4" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="E304" s="4" t="s">
         <v>1015</v>
@@ -18245,7 +18239,7 @@
         <v>1609</v>
       </c>
       <c r="D305" s="4" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="E305" s="4" t="s">
         <v>1018</v>
@@ -18280,7 +18274,7 @@
         <v>1021</v>
       </c>
       <c r="D306" s="4" t="s">
-        <v>2177</v>
+        <v>2172</v>
       </c>
       <c r="E306" s="4" t="s">
         <v>1022</v>
@@ -18315,7 +18309,7 @@
         <v>1616</v>
       </c>
       <c r="D307" s="4" t="s">
-        <v>2224</v>
+        <v>2218</v>
       </c>
       <c r="E307" s="4" t="s">
         <v>1025</v>
@@ -18350,7 +18344,7 @@
         <v>1616</v>
       </c>
       <c r="D308" s="4" t="s">
-        <v>2225</v>
+        <v>2219</v>
       </c>
       <c r="E308" s="4" t="s">
         <v>1028</v>
@@ -18385,7 +18379,7 @@
         <v>987</v>
       </c>
       <c r="D309" s="4" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E309" s="4" t="s">
         <v>1032</v>
@@ -18420,13 +18414,13 @@
         <v>1640</v>
       </c>
       <c r="D310" s="4" t="s">
-        <v>2213</v>
+        <v>2207</v>
       </c>
       <c r="E310" s="4" t="s">
         <v>1035</v>
       </c>
       <c r="F310" s="4" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="G310" s="1" t="s">
         <v>13</v>
@@ -18452,16 +18446,16 @@
         <v>2022</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D311" s="4" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="E311" s="4" t="s">
         <v>1037</v>
       </c>
       <c r="F311" s="4" t="s">
-        <v>2193</v>
+        <v>2187</v>
       </c>
       <c r="G311" s="1" t="s">
         <v>66</v>
@@ -18487,16 +18481,16 @@
         <v>2022</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D312" s="4" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="E312" s="4" t="s">
         <v>1039</v>
       </c>
       <c r="F312" s="4" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="G312" s="1" t="s">
         <v>13</v>
@@ -18522,10 +18516,10 @@
         <v>2022</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D313" s="4" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="E313" s="4" t="s">
         <v>1041</v>
@@ -18557,10 +18551,10 @@
         <v>2022</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D314" s="4" t="s">
-        <v>2226</v>
+        <v>2220</v>
       </c>
       <c r="E314" s="4" t="s">
         <v>1044</v>
@@ -18595,7 +18589,7 @@
         <v>1610</v>
       </c>
       <c r="D315" s="4" t="s">
-        <v>2227</v>
+        <v>2221</v>
       </c>
       <c r="E315" s="4" t="s">
         <v>1047</v>
@@ -18630,7 +18624,7 @@
         <v>1610</v>
       </c>
       <c r="D316" s="4" t="s">
-        <v>2178</v>
+        <v>2230</v>
       </c>
       <c r="E316" s="4" t="s">
         <v>1050</v>
@@ -18665,7 +18659,7 @@
         <v>1776</v>
       </c>
       <c r="D317" s="4" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E317" s="4" t="s">
         <v>1053</v>
@@ -18700,7 +18694,7 @@
         <v>1776</v>
       </c>
       <c r="D318" s="4" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E318" s="4" t="s">
         <v>1055</v>
@@ -18735,7 +18729,7 @@
         <v>1776</v>
       </c>
       <c r="D319" s="4" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E319" s="4" t="s">
         <v>1058</v>
@@ -18770,7 +18764,7 @@
         <v>1776</v>
       </c>
       <c r="D320" s="4" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E320" s="4" t="s">
         <v>1061</v>
@@ -18802,16 +18796,16 @@
         <v>2023</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D321" s="4" t="s">
-        <v>2214</v>
+        <v>2208</v>
       </c>
       <c r="E321" s="4" t="s">
         <v>1064</v>
       </c>
       <c r="F321" s="4" t="s">
-        <v>2195</v>
+        <v>2189</v>
       </c>
       <c r="G321" s="1" t="s">
         <v>19</v>
@@ -18837,10 +18831,10 @@
         <v>2023</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D322" s="4" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="E322" s="4" t="s">
         <v>1066</v>
@@ -18872,10 +18866,10 @@
         <v>2023</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D323" s="4" t="s">
-        <v>2179</v>
+        <v>2173</v>
       </c>
       <c r="E323" s="4" t="s">
         <v>1069</v>
@@ -18907,10 +18901,10 @@
         <v>2023</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D324" s="4" t="s">
-        <v>2179</v>
+        <v>2173</v>
       </c>
       <c r="E324" s="4" t="s">
         <v>1072</v>
@@ -18942,10 +18936,10 @@
         <v>2023</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D325" s="4" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="E325" s="4" t="s">
         <v>1075</v>
@@ -18977,10 +18971,10 @@
         <v>2023</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>1909</v>
+        <v>1782</v>
       </c>
       <c r="D326" s="4" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="E326" s="4" t="s">
         <v>1078</v>
@@ -19015,7 +19009,7 @@
         <v>1789</v>
       </c>
       <c r="D327" s="4" t="s">
-        <v>2180</v>
+        <v>2174</v>
       </c>
       <c r="E327" s="4" t="s">
         <v>1082</v>
@@ -19050,7 +19044,7 @@
         <v>1789</v>
       </c>
       <c r="D328" s="4" t="s">
-        <v>2129</v>
+        <v>2125</v>
       </c>
       <c r="E328" s="4" t="s">
         <v>1085</v>
@@ -19082,10 +19076,10 @@
         <v>2023</v>
       </c>
       <c r="C329" s="4" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D329" s="4" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E329" s="4" t="s">
         <v>1089</v>
@@ -19117,10 +19111,10 @@
         <v>2023</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D330" s="4" t="s">
-        <v>2228</v>
+        <v>2222</v>
       </c>
       <c r="E330" s="4" t="s">
         <v>1093</v>
@@ -19152,10 +19146,10 @@
         <v>2023</v>
       </c>
       <c r="C331" s="4" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D331" s="4" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="E331" s="4" t="s">
         <v>1096</v>
@@ -19190,7 +19184,7 @@
         <v>1631</v>
       </c>
       <c r="D332" s="4" t="s">
-        <v>2130</v>
+        <v>2126</v>
       </c>
       <c r="E332" s="4" t="s">
         <v>1099</v>
@@ -19225,7 +19219,7 @@
         <v>1631</v>
       </c>
       <c r="D333" s="4" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E333" s="4" t="s">
         <v>1103</v>
@@ -19260,7 +19254,7 @@
         <v>1631</v>
       </c>
       <c r="D334" s="4" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="E334" s="4" t="s">
         <v>1106</v>
@@ -19295,13 +19289,13 @@
         <v>1785</v>
       </c>
       <c r="D335" s="4" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E335" s="4" t="s">
         <v>1109</v>
       </c>
       <c r="F335" s="4" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="G335" s="1" t="s">
         <v>13</v>
@@ -19330,7 +19324,7 @@
         <v>1785</v>
       </c>
       <c r="D336" s="4" t="s">
-        <v>2131</v>
+        <v>2127</v>
       </c>
       <c r="E336" s="4" t="s">
         <v>1111</v>
@@ -19365,7 +19359,7 @@
         <v>1785</v>
       </c>
       <c r="D337" s="4" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E337" s="4" t="s">
         <v>1115</v>
@@ -19400,7 +19394,7 @@
         <v>580</v>
       </c>
       <c r="D338" s="4" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E338" s="4" t="s">
         <v>1119</v>
@@ -19435,7 +19429,7 @@
         <v>580</v>
       </c>
       <c r="D339" s="4" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E339" s="4" t="s">
         <v>1123</v>
@@ -19470,7 +19464,7 @@
         <v>1620</v>
       </c>
       <c r="D340" s="4" t="s">
-        <v>2181</v>
+        <v>2175</v>
       </c>
       <c r="E340" s="4" t="s">
         <v>1127</v>
@@ -19505,7 +19499,7 @@
         <v>1620</v>
       </c>
       <c r="D341" s="4" t="s">
-        <v>2181</v>
+        <v>2175</v>
       </c>
       <c r="E341" s="4" t="s">
         <v>1130</v>
@@ -19540,7 +19534,7 @@
         <v>1620</v>
       </c>
       <c r="D342" s="4" t="s">
-        <v>2181</v>
+        <v>2175</v>
       </c>
       <c r="E342" s="4" t="s">
         <v>1134</v>
@@ -19575,7 +19569,7 @@
         <v>1620</v>
       </c>
       <c r="D343" s="4" t="s">
-        <v>2181</v>
+        <v>2175</v>
       </c>
       <c r="E343" s="4" t="s">
         <v>1138</v>
@@ -19610,7 +19604,7 @@
         <v>1609</v>
       </c>
       <c r="D344" s="4" t="s">
-        <v>2132</v>
+        <v>2128</v>
       </c>
       <c r="E344" s="4" t="s">
         <v>1141</v>
@@ -19645,7 +19639,7 @@
         <v>1609</v>
       </c>
       <c r="D345" s="4" t="s">
-        <v>2133</v>
+        <v>2129</v>
       </c>
       <c r="E345" s="4" t="s">
         <v>1145</v>
@@ -19680,7 +19674,7 @@
         <v>1609</v>
       </c>
       <c r="D346" s="4" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="E346" s="4" t="s">
         <v>1149</v>
@@ -19715,7 +19709,7 @@
         <v>1616</v>
       </c>
       <c r="D347" s="4" t="s">
-        <v>2182</v>
+        <v>2176</v>
       </c>
       <c r="E347" s="4" t="s">
         <v>1152</v>
@@ -19750,7 +19744,7 @@
         <v>1616</v>
       </c>
       <c r="D348" s="4" t="s">
-        <v>2182</v>
+        <v>2176</v>
       </c>
       <c r="E348" s="4" t="s">
         <v>1155</v>
@@ -19785,7 +19779,7 @@
         <v>1616</v>
       </c>
       <c r="D349" s="4" t="s">
-        <v>2182</v>
+        <v>2176</v>
       </c>
       <c r="E349" s="4" t="s">
         <v>1159</v>
@@ -19817,10 +19811,10 @@
         <v>2023</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>2229</v>
+        <v>2223</v>
       </c>
       <c r="E350" s="4" t="s">
         <v>1163</v>
@@ -19852,10 +19846,10 @@
         <v>2023</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D351" s="4" t="s">
-        <v>2229</v>
+        <v>2223</v>
       </c>
       <c r="E351" s="4" t="s">
         <v>1166</v>
@@ -19890,7 +19884,7 @@
         <v>1610</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>2180</v>
+        <v>2174</v>
       </c>
       <c r="E352" s="4" t="s">
         <v>1169</v>
@@ -19925,7 +19919,7 @@
         <v>1610</v>
       </c>
       <c r="D353" s="4" t="s">
-        <v>2183</v>
+        <v>2177</v>
       </c>
       <c r="E353" s="4" t="s">
         <v>1172</v>
@@ -19960,7 +19954,7 @@
         <v>1610</v>
       </c>
       <c r="D354" s="4" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="E354" s="4" t="s">
         <v>1175</v>
@@ -19995,7 +19989,7 @@
         <v>1610</v>
       </c>
       <c r="D355" s="4" t="s">
-        <v>2184</v>
+        <v>2178</v>
       </c>
       <c r="E355" s="4" t="s">
         <v>1178</v>
@@ -20030,7 +20024,7 @@
         <v>1685</v>
       </c>
       <c r="D356" s="4" t="s">
-        <v>2185</v>
+        <v>2179</v>
       </c>
       <c r="E356" s="4" t="s">
         <v>1182</v>
@@ -20065,7 +20059,7 @@
         <v>1685</v>
       </c>
       <c r="D357" s="4" t="s">
-        <v>2185</v>
+        <v>2179</v>
       </c>
       <c r="E357" s="4" t="s">
         <v>1185</v>
@@ -20100,13 +20094,13 @@
         <v>1776</v>
       </c>
       <c r="D358" s="4" t="s">
-        <v>2134</v>
+        <v>2130</v>
       </c>
       <c r="E358" s="4" t="s">
         <v>1188</v>
       </c>
       <c r="F358" s="4" t="s">
-        <v>2186</v>
+        <v>2180</v>
       </c>
       <c r="G358" s="1" t="s">
         <v>19</v>
@@ -20135,7 +20129,7 @@
         <v>1776</v>
       </c>
       <c r="D359" s="4" t="s">
-        <v>2134</v>
+        <v>2130</v>
       </c>
       <c r="E359" s="4" t="s">
         <v>1191</v>
@@ -20170,7 +20164,7 @@
         <v>1776</v>
       </c>
       <c r="D360" s="4" t="s">
-        <v>2187</v>
+        <v>2181</v>
       </c>
       <c r="E360" s="4" t="s">
         <v>1195</v>
@@ -20205,7 +20199,7 @@
         <v>1878</v>
       </c>
       <c r="D361" s="4" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="E361" s="4" t="s">
         <v>1198</v>
@@ -20240,7 +20234,7 @@
         <v>1782</v>
       </c>
       <c r="D362" s="4" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="E362" s="4" t="s">
         <v>1201</v>
@@ -20275,7 +20269,7 @@
         <v>1782</v>
       </c>
       <c r="D363" s="4" t="s">
-        <v>2179</v>
+        <v>2173</v>
       </c>
       <c r="E363" s="4" t="s">
         <v>1205</v>
@@ -20310,7 +20304,7 @@
         <v>1782</v>
       </c>
       <c r="D364" s="4" t="s">
-        <v>2188</v>
+        <v>2182</v>
       </c>
       <c r="E364" s="4" t="s">
         <v>1209</v>
@@ -20345,7 +20339,7 @@
         <v>1790</v>
       </c>
       <c r="D365" s="4" t="s">
-        <v>2217</v>
+        <v>2211</v>
       </c>
       <c r="E365" s="4" t="s">
         <v>1213</v>
@@ -20380,7 +20374,7 @@
         <v>1790</v>
       </c>
       <c r="D366" s="4" t="s">
-        <v>2194</v>
+        <v>2188</v>
       </c>
       <c r="E366" s="4" t="s">
         <v>1217</v>
@@ -20415,7 +20409,7 @@
         <v>1790</v>
       </c>
       <c r="D367" s="4" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="E367" s="4" t="s">
         <v>1221</v>
@@ -20450,7 +20444,7 @@
         <v>1627</v>
       </c>
       <c r="D368" s="4" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="E368" s="4" t="s">
         <v>1225</v>
@@ -20485,7 +20479,7 @@
         <v>1627</v>
       </c>
       <c r="D369" s="4" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="E369" s="4" t="s">
         <v>1229</v>
@@ -20520,7 +20514,7 @@
         <v>1627</v>
       </c>
       <c r="D370" s="4" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="E370" s="4" t="s">
         <v>1233</v>
@@ -20555,7 +20549,7 @@
         <v>1789</v>
       </c>
       <c r="D371" s="4" t="s">
-        <v>2135</v>
+        <v>2131</v>
       </c>
       <c r="E371" s="4" t="s">
         <v>1236</v>
@@ -20590,7 +20584,7 @@
         <v>1789</v>
       </c>
       <c r="D372" s="4" t="s">
-        <v>2218</v>
+        <v>2212</v>
       </c>
       <c r="E372" s="4" t="s">
         <v>1240</v>
@@ -20622,7 +20616,7 @@
         <v>1789</v>
       </c>
       <c r="D373" s="4" t="s">
-        <v>2136</v>
+        <v>2132</v>
       </c>
       <c r="E373" s="4" t="s">
         <v>1243</v>
@@ -20657,7 +20651,7 @@
         <v>1789</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="E374" s="4" t="s">
         <v>1247</v>
@@ -20692,7 +20686,7 @@
         <v>1789</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>2137</v>
+        <v>2133</v>
       </c>
       <c r="E375" s="4" t="s">
         <v>1251</v>
@@ -20727,7 +20721,7 @@
         <v>1789</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>2138</v>
+        <v>2134</v>
       </c>
       <c r="E376" s="4" t="s">
         <v>1255</v>
@@ -20762,7 +20756,7 @@
         <v>1789</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="E377" s="4" t="s">
         <v>1259</v>
@@ -20797,7 +20791,7 @@
         <v>1789</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>2139</v>
+        <v>2135</v>
       </c>
       <c r="E378" s="4" t="s">
         <v>1263</v>
@@ -20829,10 +20823,10 @@
         <v>2024</v>
       </c>
       <c r="C379" s="3" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D379" s="4" t="s">
-        <v>2219</v>
+        <v>2213</v>
       </c>
       <c r="E379" s="4" t="s">
         <v>1267</v>
@@ -20864,10 +20858,10 @@
         <v>2024</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D380" s="4" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="E380" s="4" t="s">
         <v>1270</v>
@@ -20899,10 +20893,10 @@
         <v>2024</v>
       </c>
       <c r="C381" s="3" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>2215</v>
+        <v>2209</v>
       </c>
       <c r="E381" s="4" t="s">
         <v>1274</v>
@@ -20937,7 +20931,7 @@
         <v>1631</v>
       </c>
       <c r="D382" s="4" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E382" s="4" t="s">
         <v>1278</v>
@@ -20972,7 +20966,7 @@
         <v>1631</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>2140</v>
+        <v>2136</v>
       </c>
       <c r="E383" s="4" t="s">
         <v>1282</v>
@@ -21007,7 +21001,7 @@
         <v>1631</v>
       </c>
       <c r="D384" s="4" t="s">
-        <v>2216</v>
+        <v>2210</v>
       </c>
       <c r="E384" s="4" t="s">
         <v>1285</v>
@@ -21042,7 +21036,7 @@
         <v>1631</v>
       </c>
       <c r="D385" s="4" t="s">
-        <v>2141</v>
+        <v>2137</v>
       </c>
       <c r="E385" s="4" t="s">
         <v>1289</v>
@@ -21077,7 +21071,7 @@
         <v>1631</v>
       </c>
       <c r="D386" s="4" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="E386" s="4" t="s">
         <v>1293</v>
@@ -21112,7 +21106,7 @@
         <v>1631</v>
       </c>
       <c r="D387" s="4" t="s">
-        <v>2220</v>
+        <v>2214</v>
       </c>
       <c r="E387" s="4" t="s">
         <v>1296</v>
@@ -21147,7 +21141,7 @@
         <v>1631</v>
       </c>
       <c r="D388" s="4" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="E388" s="4" t="s">
         <v>1300</v>
@@ -21182,7 +21176,7 @@
         <v>1631</v>
       </c>
       <c r="D389" s="4" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="E389" s="4" t="s">
         <v>1304</v>
@@ -21217,7 +21211,7 @@
         <v>1631</v>
       </c>
       <c r="D390" s="4" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E390" s="4" t="s">
         <v>1308</v>
@@ -21252,7 +21246,7 @@
         <v>1785</v>
       </c>
       <c r="D391" s="4" t="s">
-        <v>2230</v>
+        <v>2224</v>
       </c>
       <c r="E391" s="4" t="s">
         <v>1312</v>
@@ -21287,7 +21281,7 @@
         <v>1785</v>
       </c>
       <c r="D392" s="4" t="s">
-        <v>2231</v>
+        <v>2225</v>
       </c>
       <c r="E392" s="4" t="s">
         <v>1316</v>
@@ -21322,7 +21316,7 @@
         <v>1785</v>
       </c>
       <c r="D393" s="4" t="s">
-        <v>2230</v>
+        <v>2224</v>
       </c>
       <c r="E393" s="4" t="s">
         <v>1320</v>
@@ -21357,7 +21351,7 @@
         <v>1785</v>
       </c>
       <c r="D394" s="4" t="s">
-        <v>2230</v>
+        <v>2224</v>
       </c>
       <c r="E394" s="4" t="s">
         <v>1324</v>
@@ -21392,7 +21386,7 @@
         <v>1785</v>
       </c>
       <c r="D395" s="4" t="s">
-        <v>2232</v>
+        <v>2226</v>
       </c>
       <c r="E395" s="4" t="s">
         <v>1328</v>
@@ -21427,7 +21421,7 @@
         <v>1785</v>
       </c>
       <c r="D396" s="4" t="s">
-        <v>2189</v>
+        <v>2183</v>
       </c>
       <c r="E396" s="4" t="s">
         <v>1332</v>
@@ -21462,7 +21456,7 @@
         <v>1785</v>
       </c>
       <c r="D397" s="4" t="s">
-        <v>2230</v>
+        <v>2224</v>
       </c>
       <c r="E397" s="4" t="s">
         <v>1336</v>
@@ -21497,7 +21491,7 @@
         <v>1785</v>
       </c>
       <c r="D398" s="4" t="s">
-        <v>2230</v>
+        <v>2224</v>
       </c>
       <c r="E398" s="4" t="s">
         <v>1340</v>
@@ -21529,10 +21523,10 @@
         <v>2024</v>
       </c>
       <c r="C399" s="4" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D399" s="4" t="s">
-        <v>2196</v>
+        <v>2190</v>
       </c>
       <c r="E399" s="4" t="s">
         <v>1344</v>

</xml_diff>